<commit_message>
Updated perf tests, minor updates to archeType
</commit_message>
<xml_diff>
--- a/PerformanceSheet.xlsx
+++ b/PerformanceSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtaylor\Desktop\EcsLte\EcsLte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7293693B-F6BD-46A8-AFD4-8FCAA1DDC34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90928A30-A5FC-46E2-A587-C43E1ABDDD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34980" yWindow="3210" windowWidth="21030" windowHeight="15435" tabRatio="294" xr2:uid="{37A28A76-517A-40E2-B846-E001BF2807EC}"/>
+    <workbookView xWindow="-34980" yWindow="3555" windowWidth="21030" windowHeight="15435" tabRatio="294" xr2:uid="{37A28A76-517A-40E2-B846-E001BF2807EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1CB21C-C793-4EA9-AAE0-FD14FF99BCA3}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>